<commit_message>
finished AMR scripts and meta data
</commit_message>
<xml_diff>
--- a/06. Meta data/column-meta-info-microbiological.xlsx
+++ b/06. Meta data/column-meta-info-microbiological.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\HOLIFOOD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\DATAWFSR-CHEFS\CHEFS\06. Meta data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10F2BE9-84F2-429C-8E3D-3802900AAF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570D6339-8C8C-469F-9988-C7AF85FB4830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68E513EE-DBCB-48D6-88F5-A2FC040C7E96}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{68E513EE-DBCB-48D6-88F5-A2FC040C7E96}"/>
   </bookViews>
   <sheets>
     <sheet name="meta-data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="183">
   <si>
     <t>ampc</t>
   </si>
@@ -167,9 +167,6 @@
     <t>progsampstrategy_name</t>
   </si>
   <si>
-    <t>rep_country_code</t>
-  </si>
-  <si>
     <t>rep_country_name</t>
   </si>
   <si>
@@ -512,9 +509,6 @@
     <t>CC</t>
   </si>
   <si>
-    <t>rep_Country_code</t>
-  </si>
-  <si>
     <t>rep_Country_name</t>
   </si>
   <si>
@@ -591,6 +585,9 @@
   </si>
   <si>
     <t>filename</t>
+  </si>
+  <si>
+    <t>repCountry_code</t>
   </si>
 </sst>
 </file>
@@ -655,9 +652,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -695,7 +692,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -801,7 +798,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -943,7 +940,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -953,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5364F61-3DA2-41DD-9B05-7FFE167F5DC2}">
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
@@ -967,31 +964,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
@@ -2372,13 +2369,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="B44" t="b">
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D44" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C44,catalogue!A:B,2,FALSE),VLOOKUP(A44,catalogue!A:B,2,FALSE)),"")</f>
@@ -2407,7 +2404,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -2439,13 +2436,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="b">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C46,catalogue!A:B,2,FALSE),VLOOKUP(A46,catalogue!A:B,2,FALSE)),"")</f>
@@ -2473,7 +2470,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="b">
         <v>0</v>
@@ -2505,7 +2502,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="b">
         <v>0</v>
@@ -2537,13 +2534,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
         <v>47</v>
-      </c>
-      <c r="B49" t="b">
-        <v>0</v>
-      </c>
-      <c r="C49" t="s">
-        <v>48</v>
       </c>
       <c r="D49" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C49,catalogue!A:B,2,FALSE),VLOOKUP(A49,catalogue!A:B,2,FALSE)),"")</f>
@@ -2571,13 +2568,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="b">
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C50,catalogue!A:B,2,FALSE),VLOOKUP(A50,catalogue!A:B,2,FALSE)),"")</f>
@@ -2606,7 +2603,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="b">
         <v>1</v>
@@ -2638,7 +2635,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -2670,13 +2667,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
         <v>51</v>
-      </c>
-      <c r="B53" t="b">
-        <v>0</v>
-      </c>
-      <c r="C53" t="s">
-        <v>52</v>
       </c>
       <c r="D53" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C53,catalogue!A:B,2,FALSE),VLOOKUP(A53,catalogue!A:B,2,FALSE)),"")</f>
@@ -2704,13 +2701,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C54,catalogue!A:B,2,FALSE),VLOOKUP(A54,catalogue!A:B,2,FALSE)),"")</f>
@@ -2739,7 +2736,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="b">
         <v>1</v>
@@ -2771,7 +2768,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="b">
         <v>0</v>
@@ -2803,13 +2800,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
         <v>55</v>
-      </c>
-      <c r="B57" t="b">
-        <v>0</v>
-      </c>
-      <c r="C57" t="s">
-        <v>56</v>
       </c>
       <c r="D57" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C57,catalogue!A:B,2,FALSE),VLOOKUP(A57,catalogue!A:B,2,FALSE)),"")</f>
@@ -2837,13 +2834,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="b">
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C58,catalogue!A:B,2,FALSE),VLOOKUP(A58,catalogue!A:B,2,FALSE)),"")</f>
@@ -2872,7 +2869,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="b">
         <v>1</v>
@@ -2904,13 +2901,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
         <v>58</v>
-      </c>
-      <c r="B60" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60" t="s">
-        <v>59</v>
       </c>
       <c r="D60" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C60,catalogue!A:B,2,FALSE),VLOOKUP(A60,catalogue!A:B,2,FALSE)),"")</f>
@@ -2938,13 +2935,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="b">
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C61,catalogue!A:B,2,FALSE),VLOOKUP(A61,catalogue!A:B,2,FALSE)),"")</f>
@@ -2973,7 +2970,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="b">
         <v>1</v>
@@ -3005,13 +3002,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
         <v>61</v>
-      </c>
-      <c r="B63" t="b">
-        <v>0</v>
-      </c>
-      <c r="C63" t="s">
-        <v>62</v>
       </c>
       <c r="D63" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C63,catalogue!A:B,2,FALSE),VLOOKUP(A63,catalogue!A:B,2,FALSE)),"")</f>
@@ -3039,13 +3036,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="b">
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C64,catalogue!A:B,2,FALSE),VLOOKUP(A64,catalogue!A:B,2,FALSE)),"")</f>
@@ -3074,7 +3071,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="b">
         <v>1</v>
@@ -3106,13 +3103,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
         <v>64</v>
-      </c>
-      <c r="B66" t="b">
-        <v>0</v>
-      </c>
-      <c r="C66" t="s">
-        <v>65</v>
       </c>
       <c r="D66" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C66,catalogue!A:B,2,FALSE),VLOOKUP(A66,catalogue!A:B,2,FALSE)),"")</f>
@@ -3140,13 +3137,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="b">
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D67" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C67,catalogue!A:B,2,FALSE),VLOOKUP(A67,catalogue!A:B,2,FALSE)),"")</f>
@@ -3175,7 +3172,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -3207,7 +3204,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="b">
         <v>0</v>
@@ -3239,7 +3236,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="b">
         <v>0</v>
@@ -3270,7 +3267,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" t="b">
         <v>0</v>
@@ -3301,7 +3298,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" t="b">
         <v>0</v>
@@ -3332,7 +3329,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" t="b">
         <v>1</v>
@@ -3363,7 +3360,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" t="b">
         <v>0</v>
@@ -3394,7 +3391,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" t="b">
         <v>0</v>
@@ -3426,13 +3423,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" t="b">
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
         <v>74</v>
-      </c>
-      <c r="B76" t="b">
-        <v>0</v>
-      </c>
-      <c r="C76" t="s">
-        <v>75</v>
       </c>
       <c r="D76" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C76,catalogue!A:B,2,FALSE),VLOOKUP(A76,catalogue!A:B,2,FALSE)),"")</f>
@@ -3460,13 +3457,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="b">
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D77" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C77,catalogue!A:B,2,FALSE),VLOOKUP(A77,catalogue!A:B,2,FALSE)),"")</f>
@@ -3495,7 +3492,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="b">
         <v>1</v>
@@ -3527,7 +3524,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" t="b">
         <v>0</v>
@@ -3559,7 +3556,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" t="b">
         <v>0</v>
@@ -3591,7 +3588,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="b">
         <v>0</v>
@@ -3623,7 +3620,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" t="b">
         <v>0</v>
@@ -3655,7 +3652,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" t="b">
         <v>0</v>
@@ -3687,7 +3684,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="b">
         <v>0</v>
@@ -3719,7 +3716,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="b">
         <v>0</v>
@@ -3751,7 +3748,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="b">
         <v>0</v>
@@ -3783,7 +3780,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="b">
         <v>0</v>
@@ -3814,7 +3811,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="b">
         <v>1</v>
@@ -3845,13 +3842,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="b">
         <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D89" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C89,catalogue!A:B,2,FALSE),VLOOKUP(A89,catalogue!A:B,2,FALSE)),"")</f>
@@ -3880,7 +3877,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="b">
         <v>1</v>
@@ -3912,13 +3909,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="b">
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D91" t="str">
         <f>IFERROR(IFERROR(VLOOKUP(C91,catalogue!A:B,2,FALSE),VLOOKUP(A91,catalogue!A:B,2,FALSE)),"")</f>
@@ -3946,7 +3943,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="b">
         <v>0</v>
@@ -3977,7 +3974,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="b">
         <v>0</v>
@@ -4008,7 +4005,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="b">
         <v>0</v>
@@ -4039,7 +4036,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A95" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B95" t="b">
         <v>0</v>
@@ -4086,13 +4083,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
         <v>97</v>
-      </c>
-      <c r="C1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
@@ -4100,7 +4097,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -4115,7 +4112,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -4130,7 +4127,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -4145,7 +4142,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -4160,7 +4157,7 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -4175,7 +4172,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -4190,7 +4187,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -4202,10 +4199,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -4217,10 +4214,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -4232,10 +4229,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -4247,10 +4244,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -4262,10 +4259,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -4277,10 +4274,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -4292,10 +4289,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -4307,10 +4304,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -4322,10 +4319,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -4337,10 +4334,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -4360,14 +4357,17 @@
   <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="20.8203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -4375,7 +4375,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -4383,7 +4383,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -4391,7 +4391,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -4399,7 +4399,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -4407,7 +4407,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -4415,7 +4415,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13">
         <v>13</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14">
         <v>14</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -4487,7 +4487,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -4503,7 +4503,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19">
         <v>19</v>
@@ -4519,7 +4519,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21">
         <v>21</v>
@@ -4535,7 +4535,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22">
         <v>22</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23">
         <v>23</v>
@@ -4551,7 +4551,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B24">
         <v>24</v>
@@ -4559,7 +4559,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B25">
         <v>25</v>
@@ -4567,7 +4567,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26">
         <v>26</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28">
         <v>28</v>
@@ -4591,7 +4591,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29">
         <v>29</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30">
         <v>30</v>
@@ -4607,7 +4607,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31">
         <v>31</v>
@@ -4615,7 +4615,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32">
         <v>32</v>
@@ -4623,7 +4623,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33">
         <v>33</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B34">
         <v>34</v>
@@ -4639,7 +4639,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35">
         <v>35</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36">
         <v>36</v>
@@ -4655,7 +4655,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37">
         <v>37</v>
@@ -4663,7 +4663,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38">
         <v>38</v>
@@ -4671,7 +4671,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B39">
         <v>39</v>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40">
         <v>40</v>
@@ -4687,7 +4687,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B41">
         <v>41</v>
@@ -4695,7 +4695,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42">
         <v>42</v>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43">
         <v>43</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B44">
         <v>44</v>
@@ -4719,7 +4719,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45">
         <v>45</v>
@@ -4727,7 +4727,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46">
         <v>46</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51">
         <v>51</v>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B52">
         <v>52</v>
@@ -4783,7 +4783,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B53">
         <v>53</v>
@@ -4807,7 +4807,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B56">
         <v>56</v>
@@ -4815,7 +4815,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57">
         <v>57</v>
@@ -4839,7 +4839,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60">
         <v>60</v>
@@ -4847,7 +4847,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B61">
         <v>61</v>
@@ -4855,7 +4855,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B62">
         <v>62</v>
@@ -4863,7 +4863,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63">
         <v>63</v>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B64">
         <v>64</v>
@@ -4897,7 +4897,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -4905,10 +4905,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(A2,'meta-data'!F:F,1,FALSE)</f>
@@ -4917,10 +4917,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(A3,'meta-data'!F:F,1,FALSE)</f>
@@ -4932,7 +4932,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(A4,'meta-data'!F:F,1,FALSE)</f>
@@ -4941,10 +4941,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP(A5,'meta-data'!F:F,1,FALSE)</f>
@@ -4956,7 +4956,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP(A6,'meta-data'!F:F,1,FALSE)</f>
@@ -4968,7 +4968,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP(A7,'meta-data'!F:F,1,FALSE)</f>
@@ -4977,10 +4977,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP(A8,'meta-data'!F:F,1,FALSE)</f>
@@ -4989,10 +4989,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP(A9,'meta-data'!F:F,1,FALSE)</f>
@@ -5001,10 +5001,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C10" t="str">
         <f>VLOOKUP(A10,'meta-data'!F:F,1,FALSE)</f>
@@ -5013,10 +5013,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP(A11,'meta-data'!F:F,1,FALSE)</f>
@@ -5025,10 +5025,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C12" t="str">
         <f>VLOOKUP(A12,'meta-data'!F:F,1,FALSE)</f>
@@ -5040,7 +5040,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C13" t="str">
         <f>VLOOKUP(A13,'meta-data'!F:F,1,FALSE)</f>
@@ -5049,10 +5049,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C14" t="str">
         <f>VLOOKUP(A14,'meta-data'!F:F,1,FALSE)</f>
@@ -5061,10 +5061,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C15" t="str">
         <f>VLOOKUP(A15,'meta-data'!F:F,1,FALSE)</f>
@@ -5073,10 +5073,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C16" t="str">
         <f>VLOOKUP(A16,'meta-data'!F:F,1,FALSE)</f>
@@ -5085,10 +5085,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C17" t="str">
         <f>VLOOKUP(A17,'meta-data'!F:F,1,FALSE)</f>
@@ -5097,10 +5097,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C18" t="str">
         <f>VLOOKUP(A18,'meta-data'!F:F,1,FALSE)</f>
@@ -5109,10 +5109,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C19" t="str">
         <f>VLOOKUP(A19,'meta-data'!F:F,1,FALSE)</f>
@@ -5124,7 +5124,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C20" t="str">
         <f>VLOOKUP(A20,'meta-data'!F:F,1,FALSE)</f>
@@ -5133,10 +5133,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP(A21,'meta-data'!F:F,1,FALSE)</f>
@@ -5148,7 +5148,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP(A22,'meta-data'!F:F,1,FALSE)</f>
@@ -5160,7 +5160,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C23" t="str">
         <f>VLOOKUP(A23,'meta-data'!F:F,1,FALSE)</f>
@@ -5169,10 +5169,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C24" t="str">
         <f>VLOOKUP(A24,'meta-data'!F:F,1,FALSE)</f>
@@ -5184,7 +5184,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C25" t="str">
         <f>VLOOKUP(A25,'meta-data'!F:F,1,FALSE)</f>
@@ -5196,7 +5196,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C26" t="str">
         <f>VLOOKUP(A26,'meta-data'!F:F,1,FALSE)</f>
@@ -5205,10 +5205,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C27" t="str">
         <f>VLOOKUP(A27,'meta-data'!F:F,1,FALSE)</f>
@@ -5220,7 +5220,7 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C28" t="str">
         <f>VLOOKUP(A28,'meta-data'!F:F,1,FALSE)</f>
@@ -5229,10 +5229,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C29" t="str">
         <f>VLOOKUP(A29,'meta-data'!F:F,1,FALSE)</f>
@@ -5241,10 +5241,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C30" t="str">
         <f>VLOOKUP(A30,'meta-data'!F:F,1,FALSE)</f>
@@ -5253,10 +5253,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C31" t="str">
         <f>VLOOKUP(A31,'meta-data'!F:F,1,FALSE)</f>
@@ -5265,10 +5265,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C32" t="str">
         <f>VLOOKUP(A32,'meta-data'!F:F,1,FALSE)</f>
@@ -5280,7 +5280,7 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C33" t="str">
         <f>VLOOKUP(A33,'meta-data'!F:F,1,FALSE)</f>
@@ -5289,10 +5289,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C34" t="str">
         <f>VLOOKUP(A34,'meta-data'!F:F,1,FALSE)</f>
@@ -5301,10 +5301,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C35" t="str">
         <f>VLOOKUP(A35,'meta-data'!F:F,1,FALSE)</f>
@@ -5316,7 +5316,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C36" t="str">
         <f>VLOOKUP(A36,'meta-data'!F:F,1,FALSE)</f>
@@ -5328,7 +5328,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C37" t="str">
         <f>VLOOKUP(A37,'meta-data'!F:F,1,FALSE)</f>
@@ -5337,10 +5337,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C38" t="str">
         <f>VLOOKUP(A38,'meta-data'!F:F,1,FALSE)</f>
@@ -5349,10 +5349,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C39" t="str">
         <f>VLOOKUP(A39,'meta-data'!F:F,1,FALSE)</f>
@@ -5361,10 +5361,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C40" t="str">
         <f>VLOOKUP(A40,'meta-data'!F:F,1,FALSE)</f>
@@ -5373,10 +5373,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C41" t="str">
         <f>VLOOKUP(A41,'meta-data'!F:F,1,FALSE)</f>
@@ -5385,10 +5385,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C42" t="str">
         <f>VLOOKUP(A42,'meta-data'!F:F,1,FALSE)</f>
@@ -5397,10 +5397,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C43" t="str">
         <f>VLOOKUP(A43,'meta-data'!F:F,1,FALSE)</f>
@@ -5409,10 +5409,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C44" t="str">
         <f>VLOOKUP(A44,'meta-data'!F:F,1,FALSE)</f>
@@ -5421,10 +5421,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C45" t="str">
         <f>VLOOKUP(A45,'meta-data'!F:F,1,FALSE)</f>
@@ -5433,10 +5433,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C46" t="str">
         <f>VLOOKUP(A46,'meta-data'!F:F,1,FALSE)</f>
@@ -5448,7 +5448,7 @@
         <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C47" t="str">
         <f>VLOOKUP(A47,'meta-data'!F:F,1,FALSE)</f>
@@ -5460,7 +5460,7 @@
         <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C48" t="str">
         <f>VLOOKUP(A48,'meta-data'!F:F,1,FALSE)</f>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C49" t="str">
         <f>VLOOKUP(A49,'meta-data'!F:F,1,FALSE)</f>
@@ -5481,10 +5481,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B50" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C50" t="str">
         <f>VLOOKUP(A50,'meta-data'!F:F,1,FALSE)</f>
@@ -5493,10 +5493,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C51" t="str">
         <f>VLOOKUP(A51,'meta-data'!F:F,1,FALSE)</f>
@@ -5508,7 +5508,7 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C52" t="str">
         <f>VLOOKUP(A52,'meta-data'!F:F,1,FALSE)</f>
@@ -5517,10 +5517,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C53" t="str">
         <f>VLOOKUP(A53,'meta-data'!F:F,1,FALSE)</f>
@@ -5532,7 +5532,7 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C54" t="str">
         <f>VLOOKUP(A54,'meta-data'!F:F,1,FALSE)</f>
@@ -5541,10 +5541,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C55" t="str">
         <f>VLOOKUP(A55,'meta-data'!F:F,1,FALSE)</f>
@@ -5556,7 +5556,7 @@
         <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C56" t="str">
         <f>VLOOKUP(A56,'meta-data'!F:F,1,FALSE)</f>
@@ -5565,10 +5565,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C57" t="str">
         <f>VLOOKUP(A57,'meta-data'!F:F,1,FALSE)</f>
@@ -5577,10 +5577,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>